<commit_message>
Feat: Finish print_recipy(need to be content)
</commit_message>
<xml_diff>
--- a/임베디드_재료.xlsx
+++ b/임베디드_재료.xlsx
@@ -439,7 +439,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>쌀</t>
+          <t>떡</t>
         </is>
       </c>
     </row>
@@ -449,7 +449,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>고추장</t>
+          <t>간장</t>
         </is>
       </c>
     </row>
@@ -459,7 +459,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>떡</t>
+          <t>식초</t>
         </is>
       </c>
     </row>
@@ -469,7 +469,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>고추장</t>
+          <t>간장</t>
         </is>
       </c>
     </row>
@@ -479,7 +479,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>간장</t>
+          <t>삽겹살</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>고추장</t>
+          <t>꿀</t>
         </is>
       </c>
     </row>

</xml_diff>